<commit_message>
Begun alignment correction for Flying/Not Flying experiment chromatograms.
</commit_message>
<xml_diff>
--- a/data/raw/Flying/tmp/alignment_correction.xlsx
+++ b/data/raw/Flying/tmp/alignment_correction.xlsx
@@ -20,11 +20,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="28">
   <si>
     <t xml:space="preserve">Ca_FALSE_CHC</t>
   </si>
   <si>
+    <t xml:space="preserve">Ca_TRUE_CHC</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sample</t>
   </si>
   <si>
@@ -38,6 +41,69 @@
   </si>
   <si>
     <t xml:space="preserve">up </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ib_FALSE_CHC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ib_TRUE_CHC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_21 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">down</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_27 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_40</t>
   </si>
 </sst>
 </file>
@@ -52,6 +118,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -73,6 +140,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -122,7 +190,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -130,7 +198,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -151,13 +219,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.3"/>
   </cols>
@@ -168,42 +236,383 @@
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>125</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3"/>
       <c r="B4" s="0" t="n">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>131</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>173</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3"/>
+      <c r="B10" s="0" t="n">
+        <v>187</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>173</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="0" t="n">
+        <v>209</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>173</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>173</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3"/>
+      <c r="B16" s="0" t="n">
+        <v>187</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="0" t="n">
+        <v>138</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>173</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>138</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="0" t="n">
+        <v>139</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3"/>
+      <c r="B19" s="0" t="n">
+        <v>187</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="0" t="n">
+        <v>144</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>173</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>138</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="0" t="n">
+        <v>163</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>173</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>144</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3"/>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>144</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="0" t="n">
+        <v>209</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="23">
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
     <mergeCell ref="A3:A4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="E24:E25"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Corrected alignment_correction for Flying/Not Flying experiment.
</commit_message>
<xml_diff>
--- a/data/raw/Flying/tmp/alignment_correction.xlsx
+++ b/data/raw/Flying/tmp/alignment_correction.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="36">
   <si>
     <t xml:space="preserve">Ca_FALSE_CHC</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t xml:space="preserve">Fly_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_12</t>
   </si>
   <si>
     <t xml:space="preserve">Ib_FALSE_CHC</t>
@@ -206,7 +209,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -225,10 +228,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -250,11 +249,11 @@
   </sheetPr>
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G44" activeCellId="0" sqref="G44"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.3"/>
   </cols>
@@ -418,22 +417,36 @@
       <c r="E16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E18" s="3"/>
+      <c r="F18" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="E20" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -460,7 +473,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>173</v>
@@ -469,7 +482,7 @@
         <v>9</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>99</v>
@@ -506,7 +519,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>173</v>
@@ -515,7 +528,7 @@
         <v>9</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>99</v>
@@ -546,7 +559,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>173</v>
@@ -555,7 +568,7 @@
         <v>9</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F28" s="0" t="n">
         <v>99</v>
@@ -586,7 +599,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>173</v>
@@ -595,7 +608,7 @@
         <v>9</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F31" s="0" t="n">
         <v>99</v>
@@ -638,7 +651,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>173</v>
@@ -647,7 +660,7 @@
         <v>9</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F34" s="0" t="n">
         <v>138</v>
@@ -690,7 +703,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>173</v>
@@ -699,7 +712,7 @@
         <v>9</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F37" s="0" t="n">
         <v>138</v>
@@ -730,7 +743,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>173</v>
@@ -739,7 +752,7 @@
         <v>9</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F40" s="0" t="n">
         <v>144</v>
@@ -780,7 +793,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>256</v>
@@ -789,7 +802,7 @@
         <v>6</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F44" s="0" t="n">
         <v>144</v>
@@ -818,8 +831,8 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E47" s="5" t="s">
-        <v>33</v>
+      <c r="E47" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="F47" s="0" t="n">
         <v>164</v>
@@ -829,14 +842,14 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E48" s="5"/>
+      <c r="E48" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E49" s="5"/>
+      <c r="E49" s="3"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E50" s="5" t="s">
-        <v>34</v>
+      <c r="E50" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="F50" s="0" t="n">
         <v>164</v>
@@ -846,13 +859,13 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E51" s="5"/>
+      <c r="E51" s="3"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E52" s="5"/>
+      <c r="E52" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="30">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="A3:A4"/>
@@ -862,6 +875,7 @@
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="E13:E14"/>
     <mergeCell ref="E15:E16"/>
+    <mergeCell ref="E17:E18"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="E20:G20"/>
     <mergeCell ref="A22:A24"/>

</xml_diff>